<commit_message>
updates to names: Phaenicia => Lucilia
</commit_message>
<xml_diff>
--- a/Data/Fly_community.xlsx
+++ b/Data/Fly_community.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Git in R\Urban-Ecology\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osawe\Documents\Git\Urban-Ecology\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10055FAA-460B-4575-BA9E-721ADD661E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12576" windowHeight="8472" activeTab="2"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="20904" windowHeight="12660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Site" sheetId="2" r:id="rId1"/>
@@ -18,17 +19,28 @@
     <sheet name="---" sheetId="1" r:id="rId4"/>
     <sheet name="--" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="121">
   <si>
     <t>Location</t>
   </si>
@@ -385,12 +397,18 @@
   </si>
   <si>
     <t>1:0.58</t>
+  </si>
+  <si>
+    <t>Lucilia cuprina</t>
+  </si>
+  <si>
+    <t>Lucilia sericata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,27 +459,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:R41" totalsRowShown="0">
-  <autoFilter ref="A1:R41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R41" totalsRowShown="0">
+  <autoFilter ref="A1:R41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="sn"/>
-    <tableColumn id="2" name="Date"/>
-    <tableColumn id="3" name="Location"/>
-    <tableColumn id="4" name="Longitude"/>
-    <tableColumn id="5" name="Latitude"/>
-    <tableColumn id="6" name="Collection Method"/>
-    <tableColumn id="7" name="Sex"/>
-    <tableColumn id="8" name="Musca domestica"/>
-    <tableColumn id="9" name="Stomoxys calcitrans"/>
-    <tableColumn id="10" name="Fannia canicularis"/>
-    <tableColumn id="11" name="Muscina spp."/>
-    <tableColumn id="12" name="Ophyra spp."/>
-    <tableColumn id="13" name="Phormiaa regina"/>
-    <tableColumn id="14" name="Musca sorbens"/>
-    <tableColumn id="15" name="Phaenicia sericata"/>
-    <tableColumn id="16" name="Phaenicia cuprina"/>
-    <tableColumn id="17" name="Sarcophaga spp."/>
-    <tableColumn id="18" name="Drosophila spp."/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="sn"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Date"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Location"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Longitude"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Latitude"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Collection Method"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Sex"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Musca domestica"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Stomoxys calcitrans"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Fannia canicularis"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Muscina spp."/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Ophyra spp."/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Phormiaa regina"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Musca sorbens"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Phaenicia sericata"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Phaenicia cuprina"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Sarcophaga spp."/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Drosophila spp."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -729,12 +747,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N44" sqref="N44"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,10 +796,10 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -2296,7 +2314,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:M53">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M53">
     <sortCondition ref="E2:E53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2305,12 +2323,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M36" sqref="M36"/>
+      <selection pane="bottomLeft" activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2348,10 +2366,10 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -4132,10 +4150,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -4410,7 +4428,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView zoomScale="80" workbookViewId="0">
@@ -5458,11 +5476,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changed palor to palour
</commit_message>
<xml_diff>
--- a/Data/Fly_community.xlsx
+++ b/Data/Fly_community.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osawe\Documents\Git\Urban-Ecology\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248141F2-75EC-4243-A94F-824DE3C6CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A80358-485C-40DB-910B-E21DB3F6ADCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="9615" windowWidth="38700" windowHeight="15825" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27615" yWindow="3195" windowWidth="23520" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Site" sheetId="2" r:id="rId1"/>
@@ -351,9 +351,6 @@
     <t>Kitchen (T)</t>
   </si>
   <si>
-    <t>Parlor (T)</t>
-  </si>
-  <si>
     <t>Food_site</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Parlour (T)</t>
   </si>
 </sst>
 </file>
@@ -753,9 +753,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,10 +799,10 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -1798,7 +1798,7 @@
         <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
@@ -1821,7 +1821,7 @@
         <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F35" t="s">
         <v>20</v>
@@ -1844,7 +1844,7 @@
         <v>89</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
@@ -1867,7 +1867,7 @@
         <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F37" t="s">
         <v>20</v>
@@ -1893,7 +1893,7 @@
         <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F38" t="s">
         <v>19</v>
@@ -1916,7 +1916,7 @@
         <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F39" t="s">
         <v>20</v>
@@ -1939,7 +1939,7 @@
         <v>93</v>
       </c>
       <c r="E40" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F40" t="s">
         <v>19</v>
@@ -1965,7 +1965,7 @@
         <v>93</v>
       </c>
       <c r="E41" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
@@ -1991,7 +1991,7 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F42" t="s">
         <v>19</v>
@@ -2020,7 +2020,7 @@
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F43" t="s">
         <v>20</v>
@@ -2046,7 +2046,7 @@
         <v>89</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F44" t="s">
         <v>19</v>
@@ -2072,7 +2072,7 @@
         <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F45" t="s">
         <v>20</v>
@@ -2098,7 +2098,7 @@
         <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F46" t="s">
         <v>19</v>
@@ -2124,7 +2124,7 @@
         <v>91</v>
       </c>
       <c r="E47" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
@@ -2153,7 +2153,7 @@
         <v>91</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F48" t="s">
         <v>19</v>
@@ -2182,7 +2182,7 @@
         <v>91</v>
       </c>
       <c r="E49" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F49" t="s">
         <v>20</v>
@@ -2214,7 +2214,7 @@
         <v>100</v>
       </c>
       <c r="E50" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F50" t="s">
         <v>19</v>
@@ -2243,7 +2243,7 @@
         <v>100</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F51" t="s">
         <v>20</v>
@@ -2272,7 +2272,7 @@
         <v>98</v>
       </c>
       <c r="E52" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F52" t="s">
         <v>19</v>
@@ -2298,7 +2298,7 @@
         <v>98</v>
       </c>
       <c r="E53" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F53" t="s">
         <v>20</v>
@@ -2330,7 +2330,7 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
@@ -2342,7 +2342,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2369,10 +2369,10 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -4156,7 +4156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -4168,10 +4168,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
         <v>43</v>
@@ -4180,13 +4180,13 @@
         <v>42</v>
       </c>
       <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
-        <v>108</v>
-      </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4203,7 +4203,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -4224,7 +4224,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G15" si="0">SUM(C3:D3)</f>
@@ -4245,7 +4245,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -4266,7 +4266,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -4287,7 +4287,7 @@
         <v>148</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6">
         <v>0.58299999999999996</v>
@@ -4308,7 +4308,7 @@
         <v>202</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -4329,7 +4329,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -4350,7 +4350,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -4371,7 +4371,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -4392,7 +4392,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -4413,7 +4413,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12">
         <v>0.16200000000000001</v>
@@ -4434,7 +4434,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -4455,7 +4455,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F14">
         <v>0.57099999999999995</v>
@@ -4476,7 +4476,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>

</xml_diff>